<commit_message>
removing the yr20-yr28 from ivreg2
</commit_message>
<xml_diff>
--- a/Output/2.2_tests.xlsx
+++ b/Output/2.2_tests.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="230" documentId="11_B35946AFCBE7F8494D0E1203ED430AB47004112B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77780F44-9F0C-4BF0-8C08-854F0D3CDA24}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Spec 1 - Base" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Spec 3 - Location Controls" sheetId="3" r:id="rId3"/>
     <sheet name="Spec 4 - ALL Controls" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="147">
   <si>
     <t>Conclusion</t>
   </si>
@@ -254,6 +254,216 @@
   </si>
   <si>
     <t>Fail to reject</t>
+  </si>
+  <si>
+    <t>Test of restrictions for Specification 1 - Base</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Anderson LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Sargan overidentification statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Kleibergen-Papp LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Hansen J-statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of restrictions for Specification 2 - Age Controls</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Anderson LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Sargan overidentification statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Kleibergen-Papp LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Hansen J-statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>NOTE: Partial option used for ageq and agesq</t>
+  </si>
+  <si>
+    <t>Test of restrictions for Specification 3 - Location and demographic controls</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Anderson LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Sargan overidentification statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Kleibergen-Papp LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Hansen J-statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of restrictions for Specification 4 - All Controls</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Anderson LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Sargan overidentification statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test for Underidentification (i.e. Rank Condition)</t>
+  </si>
+  <si>
+    <t>Underidentification test Kleibergen-Papp LM statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>Test of Overidentifying restrictions</t>
+  </si>
+  <si>
+    <t>Hansen J-statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>NOTE: Partial option used for ageq and agesq</t>
   </si>
 </sst>
 </file>
@@ -264,7 +474,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -289,6 +499,46 @@
       <sz val="16"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -304,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -448,38 +698,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,36 +1091,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="44.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.90625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="12.36328125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="1" ht="21">
+      <c r="A1" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" s="19"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="D4" s="6">
         <v>147.16418432615586</v>
@@ -835,58 +1129,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" s="19"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="D5" s="7">
-        <v>2.1287181421362503E-17</v>
+        <v>2.1287181421362503e-17</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="19"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D6" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7" s="19"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9" s="19"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="D9" s="6">
         <v>25.439384291590066</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10" s="19"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="D10" s="7">
         <v>0.65526097970426533</v>
@@ -895,88 +1189,88 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11" s="19"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="D11" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15" s="20"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D15" s="6">
         <v>143.86320956552197</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16" s="20"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D16" s="7">
-        <v>8.1140489831002152E-17</v>
+        <v>8.1140489831002152e-17</v>
       </c>
       <c r="F16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17" s="20"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="D17" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18" s="20"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20" s="20"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="D20" s="6">
         <v>24.652962719164812</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21" s="20"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="D21" s="7">
         <v>0.69612399482680343</v>
@@ -985,11 +1279,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22" s="20"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="D22" s="11">
         <v>29</v>
@@ -1015,87 +1309,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="44.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.90625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="12.36328125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="1" ht="21">
+      <c r="A1" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" s="19"/>
       <c r="B4" s="4"/>
       <c r="C4" s="12" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="D4" s="6">
         <v>45.17819392523522</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" s="19"/>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="D5" s="7">
-        <v>2.1162455189007275E-2</v>
+        <v>0.021162455189007275</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="19"/>
       <c r="B6" s="4"/>
       <c r="C6" s="12" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="D6" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7" s="19"/>
       <c r="B7" s="4"/>
       <c r="C7" s="12"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9" s="19"/>
       <c r="B9" s="4"/>
       <c r="C9" s="12" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="D9" s="6">
         <v>22.853371913443105</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10" s="19"/>
       <c r="B10" s="4"/>
       <c r="C10" s="12" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="D10" s="7">
         <v>0.64122858282926742</v>
@@ -1104,88 +1398,88 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11" s="19"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="D11" s="11">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.5" customHeight="1">
+    <row r="14" ht="14.5" customHeight="true">
       <c r="A14" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15" s="21"/>
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="D15" s="6">
         <v>44.544686241202307</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16" s="21"/>
       <c r="B16" s="4"/>
       <c r="C16" s="12" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="D16" s="7">
-        <v>2.4520908954435403E-2</v>
+        <v>0.024520908954435403</v>
       </c>
       <c r="F16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17" s="21"/>
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="D17" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18" s="21"/>
       <c r="B18" s="4"/>
       <c r="C18" s="12"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19" s="21"/>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20" s="21"/>
       <c r="B20" s="4"/>
       <c r="C20" s="12" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="D20" s="6">
         <v>22.467148104673932</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21" s="21"/>
       <c r="B21" s="4"/>
       <c r="C21" s="12" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="D21" s="7">
         <v>0.71327881228657186</v>
@@ -1194,19 +1488,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22" s="21"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="D22" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1229,87 +1523,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="44.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.90625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="10.36328125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="1" ht="21">
+      <c r="A1" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" s="21"/>
       <c r="B4" s="4"/>
       <c r="C4" s="13" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="D4" s="6">
         <v>142.38126901314712</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" s="21"/>
       <c r="B5" s="4"/>
       <c r="C5" s="13" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="D5" s="7">
-        <v>1.4761489456985893E-16</v>
+        <v>1.4761489456985893e-16</v>
       </c>
       <c r="F5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="21"/>
       <c r="B6" s="4"/>
       <c r="C6" s="13" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="D6" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
       <c r="C7" s="13"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9" s="21"/>
       <c r="B9" s="4"/>
       <c r="C9" s="13" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="D9" s="6">
         <v>22.487002087848161</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10" s="21"/>
       <c r="B10" s="4"/>
       <c r="C10" s="13" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="D10" s="7">
         <v>0.79947905195913571</v>
@@ -1318,88 +1612,88 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11" s="21"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="D11" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15" s="19"/>
       <c r="B15" s="4"/>
       <c r="C15" s="13" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="D15" s="6">
         <v>138.56532257415745</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16" s="19"/>
       <c r="B16" s="4"/>
       <c r="C16" s="13" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="D16" s="7">
-        <v>6.8452964410191782E-16</v>
+        <v>6.8452964410191782e-16</v>
       </c>
       <c r="F16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17" s="19"/>
       <c r="B17" s="4"/>
       <c r="C17" s="13" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="D17" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="13"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20" s="19"/>
       <c r="B20" s="4"/>
       <c r="C20" s="13" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="D20" s="6">
         <v>21.979086781149128</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="13" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="D21" s="7">
         <v>0.82105432910338161</v>
@@ -1408,11 +1702,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22" s="19"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="D22" s="11">
         <v>29</v>
@@ -1438,86 +1732,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="44.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.90625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="1" ht="21">
+      <c r="A1" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4" s="21"/>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="D4" s="6">
         <v>45.16679758182584</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5" s="21"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="D5" s="7">
-        <v>2.1218993868043733E-2</v>
+        <v>0.021218993868043733</v>
       </c>
       <c r="F5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6" s="21"/>
       <c r="B6" s="4"/>
       <c r="C6" s="14" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D6" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7" s="21"/>
       <c r="B7" s="4"/>
       <c r="C7" s="14"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9" s="21"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="D9" s="6">
         <v>19.298805097513636</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10" s="21"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="D10" s="7">
         <v>0.82356923268227189</v>
@@ -1526,88 +1820,88 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11" s="21"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="D11" s="11">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15" s="19"/>
       <c r="B15" s="4"/>
       <c r="C15" s="14" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="D15" s="6">
         <v>44.193116706925075</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16" s="19"/>
       <c r="B16" s="4"/>
       <c r="C16" s="14" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="D16" s="7">
-        <v>2.6585482181493775E-2</v>
+        <v>0.026585482181493775</v>
       </c>
       <c r="F16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17" s="19"/>
       <c r="B17" s="4"/>
       <c r="C17" s="14" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="D17" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="14"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20" s="19"/>
       <c r="B20" s="4"/>
       <c r="C20" s="14" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="D20" s="6">
         <v>19.183880336179403</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="14" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="D21" s="7">
         <v>0.86320387112231778</v>
@@ -1616,19 +1910,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22" s="19"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="D22" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="B23" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>